<commit_message>
Modify the name - Cutaneous T-cell Lymphoma
</commit_message>
<xml_diff>
--- a/input/phenotype_microbiome_dog.xlsx
+++ b/input/phenotype_microbiome_dog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\AppData\Roaming\MobaXterm\slash\RemoteFiles\525916_2_10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\AppData\Roaming\MobaXterm\slash\RemoteFiles\853422_5_35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097BFD8D-6048-4D21-A417-8669CBA782EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1504414-66F0-478F-B87C-064CC6037914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49575" yWindow="2610" windowWidth="22425" windowHeight="585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="49680" yWindow="3015" windowWidth="20685" windowHeight="585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="5" r:id="rId1"/>
@@ -554,9 +554,6 @@
     <t>s__Chlamydophila_avium</t>
   </si>
   <si>
-    <t>Cutaneous T‐cell Lymphoma</t>
-  </si>
-  <si>
     <t>Chronic Arthritis</t>
   </si>
   <si>
@@ -870,6 +867,10 @@
   </si>
   <si>
     <t>Oscillibacter valericigenes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cutaneous T-cell Lymphoma</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1683,8 +1684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8871BB2B-37C0-44CD-B7A8-BCB5971E399A}">
   <dimension ref="A1:E1076"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A243" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H251" sqref="H251"/>
+    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H210" sqref="H210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2705,10 +2706,10 @@
         <v>95</v>
       </c>
       <c r="B68" s="58" t="s">
+        <v>210</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="9" t="s">
@@ -2723,7 +2724,7 @@
         <v>100</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="9" t="s">
@@ -2885,10 +2886,10 @@
         <v>103</v>
       </c>
       <c r="B80" s="65" t="s">
+        <v>251</v>
+      </c>
+      <c r="C80" s="65" t="s">
         <v>252</v>
-      </c>
-      <c r="C80" s="65" t="s">
-        <v>253</v>
       </c>
       <c r="D80" s="13"/>
       <c r="E80" s="66" t="s">
@@ -2900,10 +2901,10 @@
         <v>103</v>
       </c>
       <c r="B81" s="65" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C81" s="65" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D81" s="13"/>
       <c r="E81" s="66" t="s">
@@ -2915,10 +2916,10 @@
         <v>103</v>
       </c>
       <c r="B82" s="65" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C82" s="65" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D82" s="13"/>
       <c r="E82" s="66" t="s">
@@ -2930,10 +2931,10 @@
         <v>103</v>
       </c>
       <c r="B83" s="65" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C83" s="65" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D83" s="13"/>
       <c r="E83" s="66" t="s">
@@ -2945,10 +2946,10 @@
         <v>103</v>
       </c>
       <c r="B84" s="65" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C84" s="65" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D84" s="13"/>
       <c r="E84" s="66" t="s">
@@ -2960,10 +2961,10 @@
         <v>103</v>
       </c>
       <c r="B85" s="65" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C85" s="65" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D85" s="13"/>
       <c r="E85" s="66" t="s">
@@ -3320,10 +3321,10 @@
         <v>120</v>
       </c>
       <c r="B109" s="67" t="s">
+        <v>258</v>
+      </c>
+      <c r="C109" s="67" t="s">
         <v>259</v>
-      </c>
-      <c r="C109" s="67" t="s">
-        <v>260</v>
       </c>
       <c r="D109" s="19"/>
       <c r="E109" s="68" t="s">
@@ -3332,13 +3333,13 @@
     </row>
     <row r="110" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B110" s="41" t="s">
         <v>101</v>
       </c>
       <c r="C110" s="41" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D110" s="19"/>
       <c r="E110" s="60" t="s">
@@ -3347,7 +3348,7 @@
     </row>
     <row r="111" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B111" s="39" t="s">
         <v>68</v>
@@ -3362,7 +3363,7 @@
     </row>
     <row r="112" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B112" s="39" t="s">
         <v>68</v>
@@ -3377,7 +3378,7 @@
     </row>
     <row r="113" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B113" s="39" t="s">
         <v>55</v>
@@ -3392,7 +3393,7 @@
     </row>
     <row r="114" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B114" s="41" t="s">
         <v>48</v>
@@ -3407,13 +3408,13 @@
     </row>
     <row r="115" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B115" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="C115" s="13" t="s">
         <v>215</v>
-      </c>
-      <c r="C115" s="13" t="s">
-        <v>216</v>
       </c>
       <c r="D115" s="13"/>
       <c r="E115" s="27" t="s">
@@ -3422,13 +3423,13 @@
     </row>
     <row r="116" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B116" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="C116" s="13" t="s">
         <v>217</v>
-      </c>
-      <c r="C116" s="13" t="s">
-        <v>218</v>
       </c>
       <c r="D116" s="13"/>
       <c r="E116" s="27" t="s">
@@ -3437,13 +3438,13 @@
     </row>
     <row r="117" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B117" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="C117" s="19" t="s">
         <v>275</v>
-      </c>
-      <c r="C117" s="19" t="s">
-        <v>276</v>
       </c>
       <c r="D117" s="19"/>
       <c r="E117" s="14" t="s">
@@ -4164,10 +4165,10 @@
         <v>145</v>
       </c>
       <c r="B165" s="65" t="s">
+        <v>207</v>
+      </c>
+      <c r="C165" s="69" t="s">
         <v>208</v>
-      </c>
-      <c r="C165" s="69" t="s">
-        <v>209</v>
       </c>
       <c r="D165" s="22"/>
       <c r="E165" s="70" t="s">
@@ -4179,10 +4180,10 @@
         <v>145</v>
       </c>
       <c r="B166" s="65" t="s">
+        <v>175</v>
+      </c>
+      <c r="C166" s="69" t="s">
         <v>176</v>
-      </c>
-      <c r="C166" s="69" t="s">
-        <v>177</v>
       </c>
       <c r="D166" s="22"/>
       <c r="E166" s="70" t="s">
@@ -4194,10 +4195,10 @@
         <v>145</v>
       </c>
       <c r="B167" s="67" t="s">
+        <v>260</v>
+      </c>
+      <c r="C167" s="71" t="s">
         <v>261</v>
-      </c>
-      <c r="C167" s="71" t="s">
-        <v>262</v>
       </c>
       <c r="D167" s="34"/>
       <c r="E167" s="72" t="s">
@@ -4344,10 +4345,10 @@
         <v>148</v>
       </c>
       <c r="B177" s="65" t="s">
+        <v>262</v>
+      </c>
+      <c r="C177" s="65" t="s">
         <v>263</v>
-      </c>
-      <c r="C177" s="65" t="s">
-        <v>264</v>
       </c>
       <c r="D177" s="13"/>
       <c r="E177" s="66" t="s">
@@ -4663,7 +4664,7 @@
         <v>156</v>
       </c>
       <c r="B198" s="21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C198" s="13" t="s">
         <v>162</v>
@@ -4678,7 +4679,7 @@
         <v>156</v>
       </c>
       <c r="B199" s="21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C199" s="13" t="s">
         <v>163</v>
@@ -4813,7 +4814,7 @@
         <v>166</v>
       </c>
       <c r="B208" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C208" s="13" t="s">
         <v>169</v>
@@ -4828,7 +4829,7 @@
         <v>166</v>
       </c>
       <c r="B209" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C209" s="13" t="s">
         <v>170</v>
@@ -4843,7 +4844,7 @@
         <v>166</v>
       </c>
       <c r="B210" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C210" s="25" t="s">
         <v>171</v>
@@ -4855,13 +4856,13 @@
     </row>
     <row r="211" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="20" t="s">
-        <v>172</v>
+        <v>277</v>
       </c>
       <c r="B211" s="50" t="s">
+        <v>220</v>
+      </c>
+      <c r="C211" s="50" t="s">
         <v>221</v>
-      </c>
-      <c r="C211" s="50" t="s">
-        <v>222</v>
       </c>
       <c r="D211" s="13"/>
       <c r="E211" s="27" t="s">
@@ -4870,13 +4871,13 @@
     </row>
     <row r="212" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="20" t="s">
-        <v>172</v>
+        <v>277</v>
       </c>
       <c r="B212" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="C212" s="50" t="s">
         <v>223</v>
-      </c>
-      <c r="C212" s="50" t="s">
-        <v>224</v>
       </c>
       <c r="D212" s="13"/>
       <c r="E212" s="27" t="s">
@@ -4884,8 +4885,8 @@
       </c>
     </row>
     <row r="213" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A213" s="23" t="s">
-        <v>172</v>
+      <c r="A213" s="20" t="s">
+        <v>277</v>
       </c>
       <c r="B213" s="34" t="s">
         <v>28</v>
@@ -4900,13 +4901,13 @@
     </row>
     <row r="214" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B214" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B214" s="4" t="s">
+      <c r="C214" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="C214" s="4" t="s">
-        <v>175</v>
       </c>
       <c r="D214" s="4"/>
       <c r="E214" s="9" t="s">
@@ -4915,13 +4916,13 @@
     </row>
     <row r="215" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B215" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C215" s="4" t="s">
         <v>176</v>
-      </c>
-      <c r="C215" s="4" t="s">
-        <v>177</v>
       </c>
       <c r="D215" s="4"/>
       <c r="E215" s="9" t="s">
@@ -4930,7 +4931,7 @@
     </row>
     <row r="216" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B216" s="4" t="s">
         <v>109</v>
@@ -4945,7 +4946,7 @@
     </row>
     <row r="217" spans="1:5" ht="63" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B217" s="4" t="s">
         <v>109</v>
@@ -4960,7 +4961,7 @@
     </row>
     <row r="218" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B218" s="4" t="s">
         <v>109</v>
@@ -4975,7 +4976,7 @@
     </row>
     <row r="219" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B219" s="7" t="s">
         <v>96</v>
@@ -4990,7 +4991,7 @@
     </row>
     <row r="220" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A220" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B220" s="49" t="s">
         <v>165</v>
@@ -5005,7 +5006,7 @@
     </row>
     <row r="221" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B221" s="13" t="s">
         <v>90</v>
@@ -5020,7 +5021,7 @@
     </row>
     <row r="222" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B222" s="13" t="s">
         <v>90</v>
@@ -5035,7 +5036,7 @@
     </row>
     <row r="223" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B223" s="13" t="s">
         <v>90</v>
@@ -5050,7 +5051,7 @@
     </row>
     <row r="224" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B224" s="13" t="s">
         <v>90</v>
@@ -5065,7 +5066,7 @@
     </row>
     <row r="225" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B225" s="13" t="s">
         <v>109</v>
@@ -5080,7 +5081,7 @@
     </row>
     <row r="226" spans="1:5" ht="63" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B226" s="13" t="s">
         <v>109</v>
@@ -5095,7 +5096,7 @@
     </row>
     <row r="227" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B227" s="13" t="s">
         <v>109</v>
@@ -5110,13 +5111,13 @@
     </row>
     <row r="228" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B228" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C228" s="13" t="s">
         <v>227</v>
-      </c>
-      <c r="C228" s="13" t="s">
-        <v>228</v>
       </c>
       <c r="D228" s="13"/>
       <c r="E228" s="27" t="s">
@@ -5125,7 +5126,7 @@
     </row>
     <row r="229" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B229" s="13" t="s">
         <v>101</v>
@@ -5140,13 +5141,13 @@
     </row>
     <row r="230" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A230" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B230" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="C230" s="13" t="s">
         <v>229</v>
-      </c>
-      <c r="C230" s="13" t="s">
-        <v>230</v>
       </c>
       <c r="D230" s="26" t="s">
         <v>125</v>
@@ -5157,13 +5158,13 @@
     </row>
     <row r="231" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B231" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C231" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D231" s="13"/>
       <c r="E231" s="27" t="s">
@@ -5172,13 +5173,13 @@
     </row>
     <row r="232" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B232" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C232" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D232" s="13"/>
       <c r="E232" s="27" t="s">
@@ -5187,13 +5188,13 @@
     </row>
     <row r="233" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B233" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C233" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D233" s="13"/>
       <c r="E233" s="27" t="s">
@@ -5202,13 +5203,13 @@
     </row>
     <row r="234" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B234" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C234" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D234" s="13"/>
       <c r="E234" s="27" t="s">
@@ -5217,13 +5218,13 @@
     </row>
     <row r="235" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B235" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C235" s="13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D235" s="13"/>
       <c r="E235" s="27" t="s">
@@ -5232,13 +5233,13 @@
     </row>
     <row r="236" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B236" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C236" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D236" s="13"/>
       <c r="E236" s="27" t="s">
@@ -5247,13 +5248,13 @@
     </row>
     <row r="237" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B237" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C237" s="13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D237" s="13"/>
       <c r="E237" s="27" t="s">
@@ -5262,13 +5263,13 @@
     </row>
     <row r="238" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B238" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C238" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D238" s="13"/>
       <c r="E238" s="27" t="s">
@@ -5277,13 +5278,13 @@
     </row>
     <row r="239" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A239" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B239" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C239" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D239" s="13"/>
       <c r="E239" s="27" t="s">
@@ -5292,13 +5293,13 @@
     </row>
     <row r="240" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B240" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C240" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D240" s="13"/>
       <c r="E240" s="27" t="s">
@@ -5307,13 +5308,13 @@
     </row>
     <row r="241" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B241" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C241" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D241" s="13"/>
       <c r="E241" s="27" t="s">
@@ -5322,13 +5323,13 @@
     </row>
     <row r="242" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B242" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C242" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D242" s="13"/>
       <c r="E242" s="27" t="s">
@@ -5337,13 +5338,13 @@
     </row>
     <row r="243" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B243" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C243" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D243" s="13"/>
       <c r="E243" s="27" t="s">
@@ -5352,13 +5353,13 @@
     </row>
     <row r="244" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B244" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C244" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D244" s="13"/>
       <c r="E244" s="27" t="s">
@@ -5367,13 +5368,13 @@
     </row>
     <row r="245" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B245" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C245" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D245" s="13"/>
       <c r="E245" s="27" t="s">
@@ -5382,13 +5383,13 @@
     </row>
     <row r="246" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B246" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C246" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D246" s="13"/>
       <c r="E246" s="27" t="s">
@@ -5397,13 +5398,13 @@
     </row>
     <row r="247" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B247" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C247" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D247" s="13"/>
       <c r="E247" s="27" t="s">
@@ -5412,13 +5413,13 @@
     </row>
     <row r="248" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B248" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C248" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D248" s="13"/>
       <c r="E248" s="27" t="s">
@@ -5427,13 +5428,13 @@
     </row>
     <row r="249" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B249" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C249" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D249" s="13"/>
       <c r="E249" s="27" t="s">
@@ -5442,13 +5443,13 @@
     </row>
     <row r="250" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B250" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C250" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D250" s="13"/>
       <c r="E250" s="27" t="s">
@@ -5457,13 +5458,13 @@
     </row>
     <row r="251" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B251" s="19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C251" s="19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D251" s="19"/>
       <c r="E251" s="14" t="s">
@@ -5472,13 +5473,13 @@
     </row>
     <row r="252" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B252" s="65" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C252" s="65" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D252" s="13"/>
       <c r="E252" s="66" t="s">
@@ -5487,13 +5488,13 @@
     </row>
     <row r="253" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A253" s="73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B253" s="74" t="s">
+        <v>265</v>
+      </c>
+      <c r="C253" s="74" t="s">
         <v>266</v>
-      </c>
-      <c r="C253" s="74" t="s">
-        <v>267</v>
       </c>
       <c r="D253" s="13"/>
       <c r="E253" s="66" t="s">
@@ -5502,7 +5503,7 @@
     </row>
     <row r="254" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B254" s="65" t="s">
         <v>68</v>
@@ -5517,7 +5518,7 @@
     </row>
     <row r="255" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A255" s="73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B255" s="65" t="s">
         <v>68</v>
@@ -5532,7 +5533,7 @@
     </row>
     <row r="256" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B256" s="65" t="s">
         <v>90</v>
@@ -5547,7 +5548,7 @@
     </row>
     <row r="257" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" s="73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B257" s="65" t="s">
         <v>90</v>
@@ -5562,7 +5563,7 @@
     </row>
     <row r="258" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B258" s="65" t="s">
         <v>90</v>
@@ -5577,7 +5578,7 @@
     </row>
     <row r="259" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" s="73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B259" s="67" t="s">
         <v>90</v>
@@ -5592,13 +5593,13 @@
     </row>
     <row r="260" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" s="73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B260" s="65" t="s">
+        <v>207</v>
+      </c>
+      <c r="C260" s="65" t="s">
         <v>208</v>
-      </c>
-      <c r="C260" s="65" t="s">
-        <v>209</v>
       </c>
       <c r="D260" s="13"/>
       <c r="E260" s="66" t="s">
@@ -5607,13 +5608,13 @@
     </row>
     <row r="261" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" s="73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B261" s="65" t="s">
+        <v>267</v>
+      </c>
+      <c r="C261" s="65" t="s">
         <v>268</v>
-      </c>
-      <c r="C261" s="65" t="s">
-        <v>269</v>
       </c>
       <c r="D261" s="13"/>
       <c r="E261" s="66" t="s">
@@ -5622,7 +5623,7 @@
     </row>
     <row r="262" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B262" s="65" t="s">
         <v>48</v>
@@ -5637,13 +5638,13 @@
     </row>
     <row r="263" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B263" s="65" t="s">
+        <v>258</v>
+      </c>
+      <c r="C263" s="65" t="s">
         <v>259</v>
-      </c>
-      <c r="C263" s="65" t="s">
-        <v>260</v>
       </c>
       <c r="D263" s="13"/>
       <c r="E263" s="66" t="s">
@@ -5652,13 +5653,13 @@
     </row>
     <row r="264" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B264" s="67" t="s">
+        <v>181</v>
+      </c>
+      <c r="C264" s="67" t="s">
         <v>182</v>
-      </c>
-      <c r="C264" s="67" t="s">
-        <v>183</v>
       </c>
       <c r="D264" s="19"/>
       <c r="E264" s="68" t="s">
@@ -5667,13 +5668,13 @@
     </row>
     <row r="265" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B265" s="65" t="s">
+        <v>269</v>
+      </c>
+      <c r="C265" s="65" t="s">
         <v>270</v>
-      </c>
-      <c r="C265" s="65" t="s">
-        <v>271</v>
       </c>
       <c r="D265" s="13"/>
       <c r="E265" s="66" t="s">
@@ -5682,13 +5683,13 @@
     </row>
     <row r="266" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="75" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B266" s="67" t="s">
+        <v>271</v>
+      </c>
+      <c r="C266" s="67" t="s">
         <v>272</v>
-      </c>
-      <c r="C266" s="67" t="s">
-        <v>273</v>
       </c>
       <c r="D266" s="19"/>
       <c r="E266" s="68" t="s">
@@ -5697,7 +5698,7 @@
     </row>
     <row r="267" spans="1:5" ht="17.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="38" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B267" s="13" t="s">
         <v>90</v>
@@ -5712,7 +5713,7 @@
     </row>
     <row r="268" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A268" s="38" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B268" s="13" t="s">
         <v>90</v>
@@ -5727,7 +5728,7 @@
     </row>
     <row r="269" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" s="38" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B269" s="13" t="s">
         <v>90</v>
@@ -5742,7 +5743,7 @@
     </row>
     <row r="270" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A270" s="40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B270" s="19" t="s">
         <v>90</v>
@@ -5757,13 +5758,13 @@
     </row>
     <row r="271" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B271" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B271" s="4" t="s">
+      <c r="C271" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C271" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="D271" s="4"/>
       <c r="E271" s="9" t="s">
@@ -5772,13 +5773,13 @@
     </row>
     <row r="272" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B272" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B272" s="4" t="s">
-        <v>187</v>
-      </c>
       <c r="C272" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D272" s="4"/>
       <c r="E272" s="9" t="s">
@@ -5787,7 +5788,7 @@
     </row>
     <row r="273" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A273" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B273" s="4" t="s">
         <v>1</v>
@@ -5802,7 +5803,7 @@
     </row>
     <row r="274" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A274" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B274" s="4" t="s">
         <v>1</v>
@@ -5817,7 +5818,7 @@
     </row>
     <row r="275" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A275" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B275" s="4" t="s">
         <v>1</v>
@@ -5832,7 +5833,7 @@
     </row>
     <row r="276" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A276" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B276" s="4" t="s">
         <v>90</v>
@@ -5847,7 +5848,7 @@
     </row>
     <row r="277" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A277" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B277" s="4" t="s">
         <v>90</v>
@@ -5862,7 +5863,7 @@
     </row>
     <row r="278" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A278" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B278" s="4" t="s">
         <v>90</v>
@@ -5877,7 +5878,7 @@
     </row>
     <row r="279" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A279" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B279" s="4" t="s">
         <v>90</v>
@@ -5892,7 +5893,7 @@
     </row>
     <row r="280" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A280" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B280" s="4" t="s">
         <v>68</v>
@@ -5907,7 +5908,7 @@
     </row>
     <row r="281" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A281" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B281" s="4" t="s">
         <v>68</v>
@@ -5922,16 +5923,16 @@
     </row>
     <row r="282" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A282" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B282" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C282" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C282" s="4" t="s">
+      <c r="D282" s="4" t="s">
         <v>191</v>
-      </c>
-      <c r="D282" s="4" t="s">
-        <v>192</v>
       </c>
       <c r="E282" s="9" t="s">
         <v>26</v>
@@ -5939,13 +5940,13 @@
     </row>
     <row r="283" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A283" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B283" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C283" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D283" s="4"/>
       <c r="E283" s="9" t="s">
@@ -5954,13 +5955,13 @@
     </row>
     <row r="284" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B284" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C284" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D284" s="4"/>
       <c r="E284" s="9" t="s">
@@ -5969,13 +5970,13 @@
     </row>
     <row r="285" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B285" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C285" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D285" s="4"/>
       <c r="E285" s="9" t="s">
@@ -5984,13 +5985,13 @@
     </row>
     <row r="286" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A286" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B286" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C286" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D286" s="4"/>
       <c r="E286" s="9" t="s">
@@ -5999,13 +6000,13 @@
     </row>
     <row r="287" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A287" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B287" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C287" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D287" s="4"/>
       <c r="E287" s="9" t="s">
@@ -6014,13 +6015,13 @@
     </row>
     <row r="288" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A288" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B288" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C288" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D288" s="4"/>
       <c r="E288" s="9" t="s">
@@ -6029,13 +6030,13 @@
     </row>
     <row r="289" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A289" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B289" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C289" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D289" s="4"/>
       <c r="E289" s="9" t="s">
@@ -6044,13 +6045,13 @@
     </row>
     <row r="290" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A290" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B290" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C290" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D290" s="7"/>
       <c r="E290" s="11" t="s">
@@ -6059,7 +6060,7 @@
     </row>
     <row r="291" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A291" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B291" s="4" t="s">
         <v>124</v>
@@ -6074,7 +6075,7 @@
     </row>
     <row r="292" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A292" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B292" s="4" t="s">
         <v>90</v>
@@ -6089,7 +6090,7 @@
     </row>
     <row r="293" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A293" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B293" s="4" t="s">
         <v>90</v>
@@ -6104,7 +6105,7 @@
     </row>
     <row r="294" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A294" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B294" s="4" t="s">
         <v>90</v>
@@ -6119,7 +6120,7 @@
     </row>
     <row r="295" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A295" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B295" s="4" t="s">
         <v>90</v>
@@ -6134,7 +6135,7 @@
     </row>
     <row r="296" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A296" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B296" s="4" t="s">
         <v>68</v>
@@ -6149,7 +6150,7 @@
     </row>
     <row r="297" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A297" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B297" s="4" t="s">
         <v>68</v>
@@ -6164,7 +6165,7 @@
     </row>
     <row r="298" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A298" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B298" s="4" t="s">
         <v>50</v>
@@ -6179,7 +6180,7 @@
     </row>
     <row r="299" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A299" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B299" s="4" t="s">
         <v>50</v>
@@ -6194,7 +6195,7 @@
     </row>
     <row r="300" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A300" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B300" s="4" t="s">
         <v>98</v>
@@ -6209,7 +6210,7 @@
     </row>
     <row r="301" spans="1:5" ht="75.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A301" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B301" s="36" t="s">
         <v>45</v>
@@ -6226,7 +6227,7 @@
     </row>
     <row r="302" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A302" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B302" s="36" t="s">
         <v>0</v>
@@ -6241,7 +6242,7 @@
     </row>
     <row r="303" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A303" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B303" s="36" t="s">
         <v>165</v>
@@ -6256,7 +6257,7 @@
     </row>
     <row r="304" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A304" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B304" s="36" t="s">
         <v>18</v>
@@ -6271,7 +6272,7 @@
     </row>
     <row r="305" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A305" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B305" s="36" t="s">
         <v>18</v>
@@ -6286,7 +6287,7 @@
     </row>
     <row r="306" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A306" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B306" s="52" t="s">
         <v>18</v>
@@ -6301,7 +6302,7 @@
     </row>
     <row r="307" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A307" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B307" s="36" t="s">
         <v>85</v>
@@ -6316,7 +6317,7 @@
     </row>
     <row r="308" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A308" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B308" s="36" t="s">
         <v>85</v>
@@ -6331,7 +6332,7 @@
     </row>
     <row r="309" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A309" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B309" s="36" t="s">
         <v>85</v>
@@ -6346,10 +6347,10 @@
     </row>
     <row r="310" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A310" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B310" s="36" t="s">
         <v>202</v>
-      </c>
-      <c r="B310" s="36" t="s">
-        <v>203</v>
       </c>
       <c r="C310" s="36" t="s">
         <v>33</v>
@@ -6361,7 +6362,7 @@
     </row>
     <row r="311" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A311" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B311" s="54" t="s">
         <v>96</v>
@@ -6376,13 +6377,13 @@
     </row>
     <row r="312" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A312" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B312" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="C312" s="36" t="s">
         <v>204</v>
-      </c>
-      <c r="C312" s="36" t="s">
-        <v>205</v>
       </c>
       <c r="D312" s="4"/>
       <c r="E312" s="37" t="s">
@@ -6391,13 +6392,13 @@
     </row>
     <row r="313" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A313" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B313" s="36" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C313" s="36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D313" s="4"/>
       <c r="E313" s="37" t="s">
@@ -6406,7 +6407,7 @@
     </row>
     <row r="314" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A314" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B314" s="4" t="s">
         <v>18</v>
@@ -6421,7 +6422,7 @@
     </row>
     <row r="315" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A315" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B315" s="4" t="s">
         <v>18</v>
@@ -6436,7 +6437,7 @@
     </row>
     <row r="316" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A316" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B316" s="7" t="s">
         <v>18</v>
@@ -6451,13 +6452,13 @@
     </row>
     <row r="317" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A317" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B317" s="54" t="s">
         <v>207</v>
       </c>
-      <c r="B317" s="54" t="s">
+      <c r="C317" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="C317" s="4" t="s">
-        <v>209</v>
       </c>
       <c r="D317" s="4"/>
       <c r="E317" s="9" t="s">
@@ -6466,7 +6467,7 @@
     </row>
     <row r="318" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A318" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B318" s="76" t="s">
         <v>85</v>
@@ -6481,7 +6482,7 @@
     </row>
     <row r="319" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A319" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B319" s="76" t="s">
         <v>85</v>
@@ -6496,7 +6497,7 @@
     </row>
     <row r="320" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A320" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B320" s="76" t="s">
         <v>85</v>
@@ -6511,7 +6512,7 @@
     </row>
     <row r="321" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A321" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B321" s="76" t="s">
         <v>50</v>
@@ -6526,7 +6527,7 @@
     </row>
     <row r="322" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A322" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B322" s="76" t="s">
         <v>50</v>
@@ -6541,7 +6542,7 @@
     </row>
     <row r="323" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A323" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B323" s="76" t="s">
         <v>0</v>
@@ -6556,7 +6557,7 @@
     </row>
     <row r="324" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A324" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B324" s="55" t="s">
         <v>96</v>
@@ -6571,7 +6572,7 @@
     </row>
     <row r="325" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A325" s="63" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B325" s="7" t="s">
         <v>0</v>
@@ -6586,7 +6587,7 @@
     </row>
     <row r="326" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A326" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B326" s="4" t="s">
         <v>48</v>
@@ -6601,7 +6602,7 @@
     </row>
     <row r="327" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A327" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B327" s="4" t="s">
         <v>68</v>
@@ -6616,7 +6617,7 @@
     </row>
     <row r="328" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A328" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B328" s="4" t="s">
         <v>68</v>
@@ -6631,13 +6632,13 @@
     </row>
     <row r="329" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A329" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B329" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C329" s="4" t="s">
         <v>180</v>
-      </c>
-      <c r="C329" s="4" t="s">
-        <v>181</v>
       </c>
       <c r="D329" s="4"/>
       <c r="E329" s="9" t="s">
@@ -6646,10 +6647,10 @@
     </row>
     <row r="330" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A330" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B330" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C330" s="51" t="s">
         <v>125</v>
@@ -6661,13 +6662,13 @@
     </row>
     <row r="331" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A331" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B331" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C331" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="C331" s="4" t="s">
-        <v>183</v>
       </c>
       <c r="D331" s="4"/>
       <c r="E331" s="9" t="s">
@@ -6676,7 +6677,7 @@
     </row>
     <row r="332" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A332" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B332" s="4" t="s">
         <v>50</v>
@@ -6691,7 +6692,7 @@
     </row>
     <row r="333" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A333" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B333" s="4" t="s">
         <v>50</v>
@@ -6706,7 +6707,7 @@
     </row>
     <row r="334" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A334" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B334" s="4" t="s">
         <v>81</v>
@@ -6721,7 +6722,7 @@
     </row>
     <row r="335" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A335" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B335" s="4" t="s">
         <v>96</v>
@@ -6736,7 +6737,7 @@
     </row>
     <row r="336" spans="1:5" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A336" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B336" s="7" t="s">
         <v>144</v>

</xml_diff>